<commit_message>
Update navigation and styles
</commit_message>
<xml_diff>
--- a/Signals.xlsx
+++ b/Signals.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" firstSheet="12" activeTab="17"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" firstSheet="12" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="Buy 17th April" sheetId="6" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="85">
   <si>
     <t>SBI</t>
   </si>
@@ -610,7 +610,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3985,7 +3985,7 @@
   <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="A1:G2"/>
+      <selection activeCell="I5" sqref="I5:J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4599,7 +4599,7 @@
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="A1:G2"/>
+      <selection activeCell="J8" sqref="I5:J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5236,15 +5236,20 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="28.42578125" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:10">
       <c r="A1" s="2" t="s">
         <v>48</v>
       </c>
@@ -5267,29 +5272,800 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>83</v>
+        <v>10</v>
       </c>
       <c r="B2">
-        <v>959.9</v>
+        <v>818.55</v>
       </c>
       <c r="C2" s="1">
-        <v>43216.136967592596</v>
+        <v>43217.13658564815</v>
       </c>
       <c r="D2" s="4">
         <v>0.1388888888888889</v>
       </c>
       <c r="E2">
-        <v>964.2</v>
+        <v>819.5</v>
       </c>
       <c r="F2" t="str">
-        <f t="shared" ref="F2" si="0">IF(G2&gt;0, "PASS", "FAIL")</f>
+        <f t="shared" ref="F2:F32" si="0">IF(G2&gt;0, "PASS", "FAIL")</f>
         <v>PASS</v>
       </c>
       <c r="G2">
-        <f t="shared" ref="G2" si="1">SUM(E2-B2)</f>
-        <v>4.3000000000000682</v>
+        <f t="shared" ref="G2:G32" si="1">SUM(E2-B2)</f>
+        <v>0.95000000000004547</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3">
+        <v>294.10000000000002</v>
+      </c>
+      <c r="C3" s="1">
+        <v>43217.131956018522</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0.1388888888888889</v>
+      </c>
+      <c r="E3">
+        <v>294.45</v>
+      </c>
+      <c r="F3" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="G3">
+        <f t="shared" si="1"/>
+        <v>0.34999999999996589</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4">
+        <v>1134.3499999999999</v>
+      </c>
+      <c r="C4" s="1">
+        <v>43217.129872685182</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0.13194444444444445</v>
+      </c>
+      <c r="E4">
+        <v>1138.5</v>
+      </c>
+      <c r="F4" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="1"/>
+        <v>4.1500000000000909</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>40</v>
+      </c>
+      <c r="C5" s="1">
+        <v>43217.077673611115</v>
+      </c>
+      <c r="D5" s="4">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="E5">
+        <v>40.6</v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="1"/>
+        <v>0.60000000000000142</v>
+      </c>
+      <c r="I5" t="s">
+        <v>59</v>
+      </c>
+      <c r="J5">
+        <f>COUNTIF(F2:F37,"PASS")</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>306.95</v>
+      </c>
+      <c r="C6" s="1">
+        <v>43217.07640046296</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0.1076388888888889</v>
+      </c>
+      <c r="E6">
+        <v>311.25</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="1"/>
+        <v>4.3000000000000114</v>
+      </c>
+      <c r="I6" t="s">
+        <v>60</v>
+      </c>
+      <c r="J6">
+        <f>COUNTIF(F2:F37,"FAIL")</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7">
+        <v>144.19999999999999</v>
+      </c>
+      <c r="C7" s="1">
+        <v>43217.071539351855</v>
+      </c>
+      <c r="D7" s="4">
+        <v>8.6805555555555566E-2</v>
+      </c>
+      <c r="E7">
+        <v>144.94999999999999</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="1"/>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8">
+        <v>244.35</v>
+      </c>
+      <c r="C8" s="1">
+        <v>43217.05568287037</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0.50347222222222221</v>
+      </c>
+      <c r="E8">
+        <v>245.55</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="1"/>
+        <v>1.2000000000000171</v>
+      </c>
+      <c r="I8" t="s">
+        <v>72</v>
+      </c>
+      <c r="J8">
+        <f>SUM(G2:G37)</f>
+        <v>84.299999999999955</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9">
+        <v>268.05</v>
+      </c>
+      <c r="C9" s="1">
+        <v>43217.052129629628</v>
+      </c>
+      <c r="D9" s="4">
+        <v>8.6805555555555566E-2</v>
+      </c>
+      <c r="E9">
+        <v>268.75</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>0.69999999999998863</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10">
+        <v>887.6</v>
+      </c>
+      <c r="C10" s="1">
+        <v>43217.531180555554</v>
+      </c>
+      <c r="D10" s="4">
+        <v>0.53472222222222221</v>
+      </c>
+      <c r="E10">
+        <v>886.05</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="0"/>
+        <v>FAIL</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="1"/>
+        <v>-1.5500000000000682</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11">
+        <v>336.05</v>
+      </c>
+      <c r="C11" s="1">
+        <v>43217.531064814815</v>
+      </c>
+      <c r="D11" s="4">
+        <v>4.8611111111111112E-2</v>
+      </c>
+      <c r="E11">
+        <v>337.5</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="1"/>
+        <v>1.4499999999999886</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12">
+        <v>115.75</v>
+      </c>
+      <c r="C12" s="1">
+        <v>43217.527905092589</v>
+      </c>
+      <c r="D12" s="4">
+        <v>5.2083333333333336E-2</v>
+      </c>
+      <c r="E12">
+        <v>117.6</v>
+      </c>
+      <c r="F12" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="1"/>
+        <v>1.8499999999999943</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" t="s">
+        <v>84</v>
+      </c>
+      <c r="B13">
+        <v>867.2</v>
+      </c>
+      <c r="C13" s="1">
+        <v>43217.512974537036</v>
+      </c>
+      <c r="D13" s="4">
+        <v>0.51736111111111105</v>
+      </c>
+      <c r="E13">
+        <v>888.45</v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="1"/>
+        <v>21.25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" t="s">
+        <v>68</v>
+      </c>
+      <c r="B14">
+        <v>606.20000000000005</v>
+      </c>
+      <c r="C14" s="1">
+        <v>43217.510347222225</v>
+      </c>
+      <c r="D14" s="4">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="E14">
+        <v>607.4</v>
+      </c>
+      <c r="F14" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="1"/>
+        <v>1.1999999999999318</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15">
+        <v>267.39999999999998</v>
+      </c>
+      <c r="C15" s="1">
+        <v>43217.496111111112</v>
+      </c>
+      <c r="D15" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="E15">
+        <v>265.7</v>
+      </c>
+      <c r="F15" t="str">
+        <f t="shared" si="0"/>
+        <v>FAIL</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="1"/>
+        <v>-1.6999999999999886</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16">
+        <v>236.5</v>
+      </c>
+      <c r="C16" s="1">
+        <v>43217.427106481482</v>
+      </c>
+      <c r="D16" s="4">
+        <v>0.52777777777777779</v>
+      </c>
+      <c r="E16">
+        <v>237.9</v>
+      </c>
+      <c r="F16" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="1"/>
+        <v>1.4000000000000057</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17">
+        <v>1079.4000000000001</v>
+      </c>
+      <c r="C17" s="1">
+        <v>43217.402546296296</v>
+      </c>
+      <c r="D17" s="4">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="E17">
+        <v>1050</v>
+      </c>
+      <c r="F17" t="str">
+        <f t="shared" si="0"/>
+        <v>FAIL</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="1"/>
+        <v>-29.400000000000091</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18">
+        <v>444.5</v>
+      </c>
+      <c r="C18" s="1">
+        <v>43217.396192129629</v>
+      </c>
+      <c r="D18" s="4">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="E18">
+        <v>446.6</v>
+      </c>
+      <c r="F18" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="1"/>
+        <v>2.1000000000000227</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>1376.95</v>
+      </c>
+      <c r="C19" s="1">
+        <v>43217.396192129629</v>
+      </c>
+      <c r="D19" s="4">
+        <v>0.42708333333333331</v>
+      </c>
+      <c r="E19">
+        <v>1364.95</v>
+      </c>
+      <c r="F19" t="str">
+        <f t="shared" si="0"/>
+        <v>FAIL</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="1"/>
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20">
+        <v>864.65</v>
+      </c>
+      <c r="C20" s="1">
+        <v>43217.395949074074</v>
+      </c>
+      <c r="D20" s="4">
+        <v>0.42708333333333331</v>
+      </c>
+      <c r="E20">
+        <v>863.7</v>
+      </c>
+      <c r="F20" t="str">
+        <f t="shared" si="0"/>
+        <v>FAIL</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="1"/>
+        <v>-0.94999999999993179</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21">
+        <v>291.05</v>
+      </c>
+      <c r="C21" s="1">
+        <v>43217.395949074074</v>
+      </c>
+      <c r="D21" s="4">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="E21">
+        <v>290.85000000000002</v>
+      </c>
+      <c r="F21" t="str">
+        <f t="shared" si="0"/>
+        <v>FAIL</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="1"/>
+        <v>-0.19999999999998863</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22">
+        <v>1241.55</v>
+      </c>
+      <c r="C22" s="1">
+        <v>43217.395740740743</v>
+      </c>
+      <c r="D22" s="4">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E22">
+        <v>1241.45</v>
+      </c>
+      <c r="F22" t="str">
+        <f t="shared" si="0"/>
+        <v>FAIL</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="1"/>
+        <v>-9.9999999999909051E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" t="s">
+        <v>65</v>
+      </c>
+      <c r="B23">
+        <v>635.70000000000005</v>
+      </c>
+      <c r="C23" s="1">
+        <v>43217.395740740743</v>
+      </c>
+      <c r="D23" s="4">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="E23">
+        <v>637.54999999999995</v>
+      </c>
+      <c r="F23" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="1"/>
+        <v>1.8499999999999091</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24">
+        <v>997.5</v>
+      </c>
+      <c r="C24" s="1">
+        <v>43217.395624999997</v>
+      </c>
+      <c r="D24" s="4">
+        <v>0.39930555555555558</v>
+      </c>
+      <c r="E24">
+        <v>1005.8</v>
+      </c>
+      <c r="F24" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="1"/>
+        <v>8.2999999999999545</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25">
+        <v>520.85</v>
+      </c>
+      <c r="C25" s="1">
+        <v>43217.395624999997</v>
+      </c>
+      <c r="D25" s="4">
+        <v>5.2083333333333336E-2</v>
+      </c>
+      <c r="E25">
+        <v>526.20000000000005</v>
+      </c>
+      <c r="F25" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="1"/>
+        <v>5.3500000000000227</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26">
+        <v>626</v>
+      </c>
+      <c r="C26" s="1">
+        <v>43217.389421296299</v>
+      </c>
+      <c r="D26" s="4">
+        <v>0.40277777777777773</v>
+      </c>
+      <c r="E26">
+        <v>640.25</v>
+      </c>
+      <c r="F26" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="1"/>
+        <v>14.25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" t="s">
+        <v>71</v>
+      </c>
+      <c r="B27">
+        <v>1147</v>
+      </c>
+      <c r="C27" s="1">
+        <v>43217.389421296299</v>
+      </c>
+      <c r="D27" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="E27">
+        <v>1150.5</v>
+      </c>
+      <c r="F27" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="1"/>
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" t="s">
+        <v>15</v>
+      </c>
+      <c r="B28">
+        <v>753.4</v>
+      </c>
+      <c r="C28" s="1">
+        <v>43217.389421296299</v>
+      </c>
+      <c r="D28" s="4">
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="E28">
+        <v>762.5</v>
+      </c>
+      <c r="F28" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="1"/>
+        <v>9.1000000000000227</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" t="s">
+        <v>20</v>
+      </c>
+      <c r="B29">
+        <v>438</v>
+      </c>
+      <c r="C29" s="1">
+        <v>43217.389351851853</v>
+      </c>
+      <c r="D29">
+        <v>11</v>
+      </c>
+      <c r="E29">
+        <v>438</v>
+      </c>
+      <c r="F29" t="str">
+        <f t="shared" si="0"/>
+        <v>FAIL</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" t="s">
+        <v>4</v>
+      </c>
+      <c r="B30">
+        <v>510.05</v>
+      </c>
+      <c r="C30" s="1">
+        <v>43217.388611111113</v>
+      </c>
+      <c r="D30" s="4">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E30">
+        <v>520.70000000000005</v>
+      </c>
+      <c r="F30" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="1"/>
+        <v>10.650000000000034</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" t="s">
+        <v>13</v>
+      </c>
+      <c r="B31">
+        <v>626.45000000000005</v>
+      </c>
+      <c r="C31" s="1">
+        <v>43217.385879629626</v>
+      </c>
+      <c r="D31" s="4">
+        <v>0.44791666666666669</v>
+      </c>
+      <c r="E31">
+        <v>633.95000000000005</v>
+      </c>
+      <c r="F31" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="1"/>
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" t="s">
+        <v>39</v>
+      </c>
+      <c r="B32">
+        <v>847.45</v>
+      </c>
+      <c r="C32" s="1">
+        <v>43217.385833333334</v>
+      </c>
+      <c r="D32" s="4">
+        <v>0.52777777777777779</v>
+      </c>
+      <c r="E32">
+        <v>874.9</v>
+      </c>
+      <c r="F32" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="1"/>
+        <v>27.449999999999932</v>
       </c>
     </row>
   </sheetData>
@@ -5299,15 +6075,20 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="25" customWidth="1"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
+    <col min="9" max="9" width="17.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:10">
       <c r="A1" s="2" t="s">
         <v>48</v>
       </c>
@@ -5330,33 +6111,182 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>44</v>
       </c>
       <c r="B2">
-        <v>37.5</v>
+        <v>284.7</v>
       </c>
       <c r="C2" s="1">
-        <v>43216.130127314813</v>
+        <v>43217.048622685186</v>
       </c>
       <c r="D2" s="4">
-        <v>0.1388888888888889</v>
+        <v>9.375E-2</v>
       </c>
       <c r="E2">
-        <v>37.25</v>
+        <v>283.7</v>
       </c>
       <c r="F2" t="str">
-        <f t="shared" ref="F2" si="0">IF(G2&gt;0, "PASS", "FAIL")</f>
+        <f t="shared" ref="F2:F7" si="0">IF(G2&gt;0, "PASS", "FAIL")</f>
         <v>PASS</v>
       </c>
       <c r="G2">
-        <f t="shared" ref="G2" si="1">SUM(B2-E2)</f>
-        <v>0.25</v>
+        <f t="shared" ref="G2:G7" si="1">SUM(B2-E2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>16.7</v>
+      </c>
+      <c r="C3" s="1">
+        <v>43217.496111111112</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0.11805555555555557</v>
+      </c>
+      <c r="E3">
+        <v>15.95</v>
+      </c>
+      <c r="F3" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="G3">
+        <f t="shared" si="1"/>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4">
+        <v>1046.2</v>
+      </c>
+      <c r="C4" s="1">
+        <v>43217.485879629632</v>
+      </c>
+      <c r="D4" s="4">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="E4">
+        <v>1040</v>
+      </c>
+      <c r="F4" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="1"/>
+        <v>6.2000000000000455</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5">
+        <v>1361.85</v>
+      </c>
+      <c r="C5" s="1">
+        <v>43217.427222222221</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0.46875</v>
+      </c>
+      <c r="E5">
+        <v>1351</v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="1"/>
+        <v>10.849999999999909</v>
+      </c>
+      <c r="I5" t="s">
+        <v>59</v>
+      </c>
+      <c r="J5">
+        <f>COUNTIF(F2:F27,"PASS")</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6">
+        <v>794.7</v>
+      </c>
+      <c r="C6" s="1">
+        <v>43217.423576388886</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0.49305555555555558</v>
+      </c>
+      <c r="E6">
+        <v>798.9</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" si="0"/>
+        <v>FAIL</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="1"/>
+        <v>-4.1999999999999318</v>
+      </c>
+      <c r="I6" t="s">
+        <v>60</v>
+      </c>
+      <c r="J6">
+        <f>COUNTIF(F2:F27,"FAIL")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7">
+        <v>230.05</v>
+      </c>
+      <c r="C7" s="1">
+        <v>43217.403240740743</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0.13194444444444445</v>
+      </c>
+      <c r="E7">
+        <v>158.80000000000001</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="1"/>
+        <v>71.25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="I8" t="s">
+        <v>72</v>
+      </c>
+      <c r="J8">
+        <f>SUM(G4:G27)</f>
+        <v>84.100000000000023</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>